<commit_message>
feat: add multiple rows support
</commit_message>
<xml_diff>
--- a/ProductCard.xlsx
+++ b/ProductCard.xlsx
@@ -397,96 +397,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <f>key</f>
         <v>data-object</v>
       </c>
       <c r="B1" t="str">
-        <v>key</v>
-      </c>
-      <c r="C1" t="str">
-        <v>productType.key</v>
-      </c>
-      <c r="D1" t="str">
-        <v>productType.typeId</v>
-      </c>
-      <c r="E1" t="str">
-        <v>name.en-GB</v>
-      </c>
-      <c r="F1" t="str">
-        <v>slug.en-GB</v>
-      </c>
-      <c r="G1" t="str">
-        <v>attributes.Size</v>
-      </c>
-      <c r="H1" t="str">
-        <v>attributes.TipWidth</v>
-      </c>
-      <c r="I1" t="str">
-        <v>attributes.WaistWidth</v>
-      </c>
-      <c r="J1" t="str">
-        <v>attributes.TailWidth</v>
-      </c>
-      <c r="K1" t="str">
-        <v>attributes.SidecutRadius</v>
-      </c>
-      <c r="L1" t="str">
-        <v>attributes.RiderWeight</v>
-      </c>
-      <c r="M1" t="str">
-        <v>attributes.Width</v>
+        <f>snowboard108</f>
+        <v>variant</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>variant</v>
+        <f>key</f>
+        <v>data-object</v>
       </c>
       <c r="B2" t="str">
-        <v>snowboard3</v>
-      </c>
-      <c r="C2" t="str">
-        <v>snowboardTypeKey</v>
-      </c>
-      <c r="D2" t="str">
-        <v>product-type</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Ride Twinpig Snowboard 2024</v>
-      </c>
-      <c r="F2" t="str">
-        <v>snowboard3</v>
-      </c>
-      <c r="G2" t="str">
-        <v>136</v>
-      </c>
-      <c r="H2" t="str">
-        <v>287</v>
-      </c>
-      <c r="I2" t="str">
-        <v>240</v>
-      </c>
-      <c r="J2" t="str">
-        <v>287</v>
-      </c>
-      <c r="K2" t="str">
-        <v>6.2​/5.3, 5.2​/4.3, 6.2​/5.3</v>
-      </c>
-      <c r="L2" t="str">
-        <v>60-130</v>
-      </c>
-      <c r="M2" t="str">
-        <v>Regular</v>
+        <f>snowboard107</f>
+        <v>variant</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:P2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>